<commit_message>
The player can use items now with only a echo as return
</commit_message>
<xml_diff>
--- a/Eigen spel/PotionStats.xlsx
+++ b/Eigen spel/PotionStats.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Potion" sheetId="1" r:id="rId1"/>
+    <sheet name="Item stats" sheetId="2" r:id="rId2"/>
+    <sheet name="Potion stats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
   <si>
     <t>Potion</t>
   </si>
@@ -98,12 +100,6 @@
     <t>Yellow</t>
   </si>
   <si>
-    <t>50 extra gold</t>
-  </si>
-  <si>
-    <t>50 lost gold</t>
-  </si>
-  <si>
     <t>Green Potion</t>
   </si>
   <si>
@@ -132,6 +128,159 @@
   </si>
   <si>
     <t>Max HP</t>
+  </si>
+  <si>
+    <t>Pink Potion</t>
+  </si>
+  <si>
+    <t>Pink</t>
+  </si>
+  <si>
+    <t>Inc MaxHp &gt;75</t>
+  </si>
+  <si>
+    <t>Dec MaxHP &lt; 75</t>
+  </si>
+  <si>
+    <t>Items stats</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Token name</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Antenne</t>
+  </si>
+  <si>
+    <t>{Empty}</t>
+  </si>
+  <si>
+    <t>Recevier</t>
+  </si>
+  <si>
+    <t>Silincer</t>
+  </si>
+  <si>
+    <t>Decrease Atk with 5</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>GoldBar</t>
+  </si>
+  <si>
+    <t>1000 extra coins</t>
+  </si>
+  <si>
+    <t>Jerrycan</t>
+  </si>
+  <si>
+    <t>{empty}</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>KeyGY</t>
+  </si>
+  <si>
+    <t>KeyPS</t>
+  </si>
+  <si>
+    <t>KeyBK</t>
+  </si>
+  <si>
+    <t>Open Door</t>
+  </si>
+  <si>
+    <t>Paddle</t>
+  </si>
+  <si>
+    <t>Use End 1</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Use to load boat</t>
+  </si>
+  <si>
+    <t>Boat</t>
+  </si>
+  <si>
+    <t>Use to row to other side</t>
+  </si>
+  <si>
+    <t>Flare</t>
+  </si>
+  <si>
+    <t>Use for end3 and 4</t>
+  </si>
+  <si>
+    <t>Functie</t>
+  </si>
+  <si>
+    <t>1000 extra gold</t>
+  </si>
+  <si>
+    <t>250 lost gold</t>
+  </si>
+  <si>
+    <t>L_Red_potion</t>
+  </si>
+  <si>
+    <t>D_Red_potion</t>
+  </si>
+  <si>
+    <t>L_Purple_potion</t>
+  </si>
+  <si>
+    <t>D_Purple_potion</t>
+  </si>
+  <si>
+    <t>Purple_potion</t>
+  </si>
+  <si>
+    <t>L_Cyan_potion</t>
+  </si>
+  <si>
+    <t>D_Cyan_potion</t>
+  </si>
+  <si>
+    <t>L_Orange_potion</t>
+  </si>
+  <si>
+    <t>D_Orange_potion</t>
+  </si>
+  <si>
+    <t>L_Yellow_potion</t>
+  </si>
+  <si>
+    <t>D_Yellow_potion</t>
+  </si>
+  <si>
+    <t>L_Green_potion</t>
+  </si>
+  <si>
+    <t>Green_potion</t>
+  </si>
+  <si>
+    <t>D_Green_potion</t>
+  </si>
+  <si>
+    <t>L_Pink_Potion</t>
+  </si>
+  <si>
+    <t>D_Pink_Potion</t>
+  </si>
+  <si>
+    <t>Rainbow_potion</t>
   </si>
 </sst>
 </file>
@@ -492,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +786,7 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15">
         <v>40</v>
@@ -651,7 +800,7 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16">
         <v>40</v>
@@ -665,7 +814,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D18">
         <v>250</v>
@@ -679,7 +828,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D19">
         <v>250</v>
@@ -687,13 +836,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21">
         <v>350</v>
@@ -701,13 +850,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D22">
         <v>350</v>
@@ -715,13 +864,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D23">
         <v>350</v>
@@ -729,20 +878,552 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25">
-        <v>15</v>
+      <c r="D28">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>36</v>
+      </c>
+      <c r="D6">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>55</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>48</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Potions now work correct as they been used
</commit_message>
<xml_diff>
--- a/Eigen spel/PotionStats.xlsx
+++ b/Eigen spel/PotionStats.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Potion" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="88">
   <si>
     <t>Potion</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Dec HP 50</t>
   </si>
   <si>
-    <t xml:space="preserve"> INV for 5 turns</t>
-  </si>
-  <si>
     <t>Cyan Potion</t>
   </si>
   <si>
@@ -115,12 +112,6 @@
     <t>All good effects</t>
   </si>
   <si>
-    <t>wep dmg +10</t>
-  </si>
-  <si>
-    <t>wep dmg -10</t>
-  </si>
-  <si>
     <t>HP set to 1</t>
   </si>
   <si>
@@ -281,6 +272,24 @@
   </si>
   <si>
     <t>Rainbow_potion</t>
+  </si>
+  <si>
+    <t>Versterker</t>
+  </si>
+  <si>
+    <t>Security Card</t>
+  </si>
+  <si>
+    <t>SCWPC</t>
+  </si>
+  <si>
+    <t>Inc Def 80</t>
+  </si>
+  <si>
+    <t>GINB *2</t>
+  </si>
+  <si>
+    <t>GINB /2</t>
   </si>
 </sst>
 </file>
@@ -644,7 +653,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C16" sqref="C15:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,7 +739,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="D9">
         <v>45</v>
@@ -752,13 +761,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
       </c>
       <c r="D12">
         <v>30</v>
@@ -766,13 +775,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13">
         <v>30</v>
@@ -780,13 +789,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="D15">
         <v>40</v>
@@ -794,13 +803,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="D16">
         <v>40</v>
@@ -808,13 +817,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D18">
         <v>250</v>
@@ -822,13 +831,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19">
         <v>250</v>
@@ -836,13 +845,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21">
         <v>350</v>
@@ -850,13 +859,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
         <v>24</v>
       </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D22">
         <v>350</v>
@@ -864,13 +873,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="B23" t="s">
-        <v>25</v>
-      </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D23">
         <v>350</v>
@@ -878,13 +887,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D25">
         <v>780</v>
@@ -892,13 +901,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
         <v>34</v>
-      </c>
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>37</v>
       </c>
       <c r="D26">
         <v>780</v>
@@ -906,13 +915,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>27</v>
-      </c>
-      <c r="C28" t="s">
-        <v>28</v>
       </c>
       <c r="D28">
         <v>25</v>
@@ -926,10 +935,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,33 +948,37 @@
     <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -979,61 +992,73 @@
       <c r="E6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="C8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B13">
         <v>11</v>
@@ -1047,39 +1072,48 @@
       <c r="E13">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" t="s">
         <v>59</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E15" t="s">
         <v>61</v>
       </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" t="s">
-        <v>64</v>
+      <c r="F15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1087,21 +1121,21 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1118,36 +1152,36 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" t="s">
         <v>54</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1160,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,13 +1210,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1196,7 +1230,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,7 +1244,7 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1224,7 +1258,7 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1235,10 +1269,10 @@
         <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,178 +1286,179 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>53</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>55</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>